<commit_message>
Include descriptions in the input excel files.
</commit_message>
<xml_diff>
--- a/Input_Excel_Empty_Template.xlsx
+++ b/Input_Excel_Empty_Template.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fdf6d9f7afe5b85/Dokumente/Projects/CookiePlanner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3fdf6d9f7afe5b85/Dokumente/GitHub/CookiePlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{CC1EB012-5510-4942-BB14-3578F046B2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D630D8EF-4A9C-409D-89E2-89A5AAFBE9ED}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="8_{CC1EB012-5510-4942-BB14-3578F046B2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A4A9F45-9776-4738-835B-B35920F8E4A8}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{94744077-A3A9-4F9A-B4E7-4B080947AE13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{94744077-A3A9-4F9A-B4E7-4B080947AE13}"/>
   </bookViews>
   <sheets>
-    <sheet name="Recipes" sheetId="1" r:id="rId1"/>
-    <sheet name="Ingredients" sheetId="2" r:id="rId2"/>
-    <sheet name="Measures" sheetId="3" r:id="rId3"/>
-    <sheet name="Hidden_DD" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Explanation" sheetId="5" r:id="rId1"/>
+    <sheet name="Recipes" sheetId="1" r:id="rId2"/>
+    <sheet name="Ingredients" sheetId="2" r:id="rId3"/>
+    <sheet name="Measures" sheetId="3" r:id="rId4"/>
+    <sheet name="Hidden_DD" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Measures">Measures!$B$2:INDEX(Measures!$B:$B,COUNTA(Measures!$B:$B))</definedName>
@@ -39,8 +40,98 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={530C0362-7165-49A1-B4E9-D42B916D846A}</author>
+    <author>tc={916FFE48-71A8-4402-8894-806354D8F9DE}</author>
+    <author>tc={1A4F8885-D86E-45CB-A258-2113AEBDE590}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{530C0362-7165-49A1-B4E9-D42B916D846A}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Enter the recipe name. Best practice is to enter the most important recipes first as they are better visible in the app.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{916FFE48-71A8-4402-8894-806354D8F9DE}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Here you can add a free comment (e.g. book/page/URL where the recipe stems from).</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="2" shapeId="0" xr:uid="{1A4F8885-D86E-45CB-A258-2113AEBDE590}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Here you will automatically see the ingredients that you can define in the Ingredients sheet. Blanks will be treated as 0 in the app so you don't have to fill everything with 0s.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={F3F01FCA-9986-46C7-93EF-815DA4C5E34B}</author>
+    <author>tc={E276D4FA-19AD-4B77-ADDA-E9944AAF34DA}</author>
+    <author>tc={7731E2F0-AB33-4808-8C73-90925447958E}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F3F01FCA-9986-46C7-93EF-815DA4C5E34B}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Enter the ingredient names. Best practice is to enter the most important ingredients first as they are better visible in the app. These will automatically be available in the Recipes sheet.</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{E276D4FA-19AD-4B77-ADDA-E9944AAF34DA}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Enter the measure associated with the ingredient. You can only use the measures you define in the Measures sheet.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="2" shapeId="0" xr:uid="{7731E2F0-AB33-4808-8C73-90925447958E}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Select "Yes" or "No". Enter Yes for the ingredients you want to be able to scale the quantity in your app (typically egg whites and egg yolks). Enter No for all other ingredients.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D98EF8AC-B915-42C3-BA7B-08640C6B628E}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D98EF8AC-B915-42C3-BA7B-08640C6B628E}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Enter your measures (for the dropdown in the Ingredients sheet). You can also overwrite the ones predefined.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Number</t>
   </si>
@@ -86,12 +177,30 @@
   <si>
     <t>Anz.</t>
   </si>
+  <si>
+    <t>This excel sheet allows you to enter your ingredients (with associated measure) and the quantities required for your recipes.</t>
+  </si>
+  <si>
+    <t>CookiePlanner Input Excel</t>
+  </si>
+  <si>
+    <t>Please follow these steps to successfully enter your information:</t>
+  </si>
+  <si>
+    <t>1. Go to the sheet "Measures" and enter the measures you want to use (try to abbreviate where possible)</t>
+  </si>
+  <si>
+    <t>2. Go to the sheet "Ingredients" and enter your ingredients. You will need to enter all three columns for the ingredients (i.e. Name, Measure and App_Qty_Input)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Go to the sheet "Recipes" and enter your recipes with the quantities required. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +225,27 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -165,6 +295,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -180,6 +315,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Nicolas Schuler" id="{C6C2CEB5-284C-4FF2-AA21-F5E3F7B76B1D}" userId="3fdf6d9f7afe5b85" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -477,12 +618,132 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2022-05-27T14:38:19.04" personId="{C6C2CEB5-284C-4FF2-AA21-F5E3F7B76B1D}" id="{530C0362-7165-49A1-B4E9-D42B916D846A}">
+    <text>Enter the recipe name. Best practice is to enter the most important recipes first as they are better visible in the app.</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2022-05-27T14:39:29.53" personId="{C6C2CEB5-284C-4FF2-AA21-F5E3F7B76B1D}" id="{916FFE48-71A8-4402-8894-806354D8F9DE}">
+    <text>Here you can add a free comment (e.g. book/page/URL where the recipe stems from).</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2022-05-27T14:40:04.78" personId="{C6C2CEB5-284C-4FF2-AA21-F5E3F7B76B1D}" id="{1A4F8885-D86E-45CB-A258-2113AEBDE590}">
+    <text>Here you will automatically see the ingredients that you can define in the Ingredients sheet. Blanks will be treated as 0 in the app so you don't have to fill everything with 0s.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2022-05-27T14:35:24.19" personId="{C6C2CEB5-284C-4FF2-AA21-F5E3F7B76B1D}" id="{F3F01FCA-9986-46C7-93EF-815DA4C5E34B}">
+    <text>Enter the ingredient names. Best practice is to enter the most important ingredients first as they are better visible in the app. These will automatically be available in the Recipes sheet.</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2022-05-27T14:36:00.51" personId="{C6C2CEB5-284C-4FF2-AA21-F5E3F7B76B1D}" id="{E276D4FA-19AD-4B77-ADDA-E9944AAF34DA}">
+    <text>Enter the measure associated with the ingredient. You can only use the measures you define in the Measures sheet.</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2022-05-27T14:37:09.80" personId="{C6C2CEB5-284C-4FF2-AA21-F5E3F7B76B1D}" id="{7731E2F0-AB33-4808-8C73-90925447958E}">
+    <text>Select "Yes" or "No". Enter Yes for the ingredients you want to be able to scale the quantity in your app (typically egg whites and egg yolks). Enter No for all other ingredients.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2022-05-27T14:34:00.96" personId="{C6C2CEB5-284C-4FF2-AA21-F5E3F7B76B1D}" id="{D98EF8AC-B915-42C3-BA7B-08640C6B628E}">
+    <text>Enter your measures (for the dropdown in the Ingredients sheet). You can also overwrite the ones predefined.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00492FE-407B-44E8-A6B8-F171B8D0A372}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E2334D-A729-4BBD-9D03-88F5496B8E4C}">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="13"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="13"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="13"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="A4:K4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00492FE-407B-44E8-A6B8-F171B8D0A372}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:AG501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19122,7 +19383,7 @@
       <c r="AG501" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name already exists" error="This recipe name already exists. Please enter a unique recipe name!" sqref="B2:B501" xr:uid="{21E30719-209D-4F51-BA0B-C7C44F7F6ACB}">
@@ -19130,15 +19391,19 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1015BF-E329-442B-8C55-26EE09700613}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1015BF-E329-442B-8C55-26EE09700613}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:D7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19807,13 +20072,14 @@
       <c r="E101" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31" xr:uid="{E6208523-B551-4006-AD94-84F153B779F7}">
       <formula1>Measures</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -19829,12 +20095,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827DC447-6286-450E-96BD-6A65D2066FB4}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827DC447-6286-450E-96BD-6A65D2066FB4}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20012,13 +20281,14 @@
       <c r="B26" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE42862-5EDB-497F-BCB4-08979C265F90}">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>